<commit_message>
commit at the end of the day - 2020/08/12
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/out/production/resources/report/国民年金第３号被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/out/production/resources/report/国民年金第３号被保険者住所変更届.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\nts.uk\uk.pr\pr.file\nts.uk.file.pr.infra\out\production\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\nts.uk\uk.pr\pr.file\nts.uk.file.pr.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2561,9 +2561,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2670,6 +2667,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2955,7 +2955,7 @@
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
           <a:off x="576629" y="205154"/>
-          <a:ext cx="2161442" cy="922257"/>
+          <a:ext cx="2228117" cy="922257"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="227" cy="85"/>
         </a:xfrm>
@@ -9087,10 +9087,8 @@
   <cols>
     <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
     <col min="2" max="4" width="1.625" style="1"/>
-    <col min="5" max="5" width="1.625" style="1" customWidth="1"/>
-    <col min="6" max="14" width="1.625" style="1"/>
-    <col min="15" max="15" width="1.625" style="1" customWidth="1"/>
-    <col min="16" max="37" width="1.625" style="1"/>
+    <col min="5" max="5" width="2.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="37" width="1.625" style="1"/>
     <col min="38" max="38" width="1.625" style="1" customWidth="1"/>
     <col min="39" max="67" width="1.625" style="1"/>
     <col min="68" max="68" width="1.875" style="1" customWidth="1"/>
@@ -9575,19 +9573,19 @@
       <c r="D9" s="122"/>
       <c r="E9" s="80"/>
       <c r="F9" s="81"/>
-      <c r="G9" s="275" t="s">
+      <c r="G9" s="274" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="276"/>
-      <c r="I9" s="277"/>
-      <c r="J9" s="284" t="s">
+      <c r="H9" s="275"/>
+      <c r="I9" s="276"/>
+      <c r="J9" s="283" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="285"/>
-      <c r="L9" s="285"/>
-      <c r="M9" s="285"/>
-      <c r="N9" s="285"/>
-      <c r="O9" s="286"/>
+      <c r="K9" s="284"/>
+      <c r="L9" s="284"/>
+      <c r="M9" s="284"/>
+      <c r="N9" s="284"/>
+      <c r="O9" s="285"/>
       <c r="P9" s="37"/>
       <c r="Q9" s="41"/>
       <c r="R9" s="37"/>
@@ -9665,15 +9663,15 @@
       <c r="D10" s="122"/>
       <c r="E10" s="80"/>
       <c r="F10" s="81"/>
-      <c r="G10" s="278"/>
-      <c r="H10" s="279"/>
-      <c r="I10" s="280"/>
-      <c r="J10" s="287"/>
-      <c r="K10" s="288"/>
-      <c r="L10" s="288"/>
-      <c r="M10" s="288"/>
-      <c r="N10" s="288"/>
-      <c r="O10" s="289"/>
+      <c r="G10" s="277"/>
+      <c r="H10" s="278"/>
+      <c r="I10" s="279"/>
+      <c r="J10" s="286"/>
+      <c r="K10" s="287"/>
+      <c r="L10" s="287"/>
+      <c r="M10" s="287"/>
+      <c r="N10" s="287"/>
+      <c r="O10" s="288"/>
       <c r="P10" s="120"/>
       <c r="Q10" s="121"/>
       <c r="R10" s="120"/>
@@ -9747,15 +9745,15 @@
       <c r="D11" s="122"/>
       <c r="E11" s="80"/>
       <c r="F11" s="81"/>
-      <c r="G11" s="281"/>
-      <c r="H11" s="282"/>
-      <c r="I11" s="283"/>
-      <c r="J11" s="290"/>
-      <c r="K11" s="291"/>
-      <c r="L11" s="291"/>
-      <c r="M11" s="291"/>
-      <c r="N11" s="291"/>
-      <c r="O11" s="292"/>
+      <c r="G11" s="280"/>
+      <c r="H11" s="281"/>
+      <c r="I11" s="282"/>
+      <c r="J11" s="289"/>
+      <c r="K11" s="290"/>
+      <c r="L11" s="290"/>
+      <c r="M11" s="290"/>
+      <c r="N11" s="290"/>
+      <c r="O11" s="291"/>
       <c r="P11" s="39"/>
       <c r="Q11" s="42"/>
       <c r="R11" s="39"/>
@@ -9834,81 +9832,81 @@
       </c>
       <c r="H12" s="196"/>
       <c r="I12" s="197"/>
-      <c r="J12" s="284" t="s">
+      <c r="J12" s="283" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="285"/>
-      <c r="L12" s="285"/>
-      <c r="M12" s="285"/>
-      <c r="N12" s="285"/>
-      <c r="O12" s="286"/>
-      <c r="P12" s="293"/>
-      <c r="Q12" s="294"/>
-      <c r="R12" s="294"/>
-      <c r="S12" s="294"/>
-      <c r="T12" s="294"/>
-      <c r="U12" s="294"/>
-      <c r="V12" s="294"/>
-      <c r="W12" s="294"/>
-      <c r="X12" s="294"/>
-      <c r="Y12" s="294"/>
-      <c r="Z12" s="294"/>
-      <c r="AA12" s="294"/>
-      <c r="AB12" s="294"/>
-      <c r="AC12" s="294"/>
-      <c r="AD12" s="294"/>
-      <c r="AE12" s="294"/>
-      <c r="AF12" s="294"/>
-      <c r="AG12" s="294"/>
-      <c r="AH12" s="294"/>
-      <c r="AI12" s="294"/>
-      <c r="AJ12" s="294"/>
-      <c r="AK12" s="294"/>
-      <c r="AL12" s="294"/>
-      <c r="AM12" s="294"/>
-      <c r="AN12" s="294"/>
-      <c r="AO12" s="294"/>
-      <c r="AP12" s="294"/>
-      <c r="AQ12" s="294"/>
-      <c r="AR12" s="294"/>
-      <c r="AS12" s="294"/>
-      <c r="AT12" s="294"/>
-      <c r="AU12" s="294"/>
-      <c r="AV12" s="294"/>
-      <c r="AW12" s="294"/>
-      <c r="AX12" s="294"/>
-      <c r="AY12" s="294"/>
-      <c r="AZ12" s="294"/>
-      <c r="BA12" s="294"/>
-      <c r="BB12" s="294"/>
-      <c r="BC12" s="294"/>
-      <c r="BD12" s="294"/>
-      <c r="BE12" s="294"/>
-      <c r="BF12" s="294"/>
-      <c r="BG12" s="294"/>
-      <c r="BH12" s="294"/>
-      <c r="BI12" s="294"/>
-      <c r="BJ12" s="294"/>
-      <c r="BK12" s="294"/>
-      <c r="BL12" s="294"/>
-      <c r="BM12" s="294"/>
-      <c r="BN12" s="294"/>
-      <c r="BO12" s="294"/>
-      <c r="BP12" s="294"/>
-      <c r="BQ12" s="294"/>
-      <c r="BR12" s="294"/>
-      <c r="BS12" s="294"/>
-      <c r="BT12" s="294"/>
-      <c r="BU12" s="294"/>
-      <c r="BV12" s="294"/>
-      <c r="BW12" s="294"/>
-      <c r="BX12" s="294"/>
-      <c r="BY12" s="294"/>
-      <c r="BZ12" s="294"/>
-      <c r="CA12" s="294"/>
-      <c r="CB12" s="294"/>
-      <c r="CC12" s="294"/>
-      <c r="CD12" s="295"/>
+      <c r="K12" s="284"/>
+      <c r="L12" s="284"/>
+      <c r="M12" s="284"/>
+      <c r="N12" s="284"/>
+      <c r="O12" s="285"/>
+      <c r="P12" s="292"/>
+      <c r="Q12" s="293"/>
+      <c r="R12" s="293"/>
+      <c r="S12" s="293"/>
+      <c r="T12" s="293"/>
+      <c r="U12" s="293"/>
+      <c r="V12" s="293"/>
+      <c r="W12" s="293"/>
+      <c r="X12" s="293"/>
+      <c r="Y12" s="293"/>
+      <c r="Z12" s="293"/>
+      <c r="AA12" s="293"/>
+      <c r="AB12" s="293"/>
+      <c r="AC12" s="293"/>
+      <c r="AD12" s="293"/>
+      <c r="AE12" s="293"/>
+      <c r="AF12" s="293"/>
+      <c r="AG12" s="293"/>
+      <c r="AH12" s="293"/>
+      <c r="AI12" s="293"/>
+      <c r="AJ12" s="293"/>
+      <c r="AK12" s="293"/>
+      <c r="AL12" s="293"/>
+      <c r="AM12" s="293"/>
+      <c r="AN12" s="293"/>
+      <c r="AO12" s="293"/>
+      <c r="AP12" s="293"/>
+      <c r="AQ12" s="293"/>
+      <c r="AR12" s="293"/>
+      <c r="AS12" s="293"/>
+      <c r="AT12" s="293"/>
+      <c r="AU12" s="293"/>
+      <c r="AV12" s="293"/>
+      <c r="AW12" s="293"/>
+      <c r="AX12" s="293"/>
+      <c r="AY12" s="293"/>
+      <c r="AZ12" s="293"/>
+      <c r="BA12" s="293"/>
+      <c r="BB12" s="293"/>
+      <c r="BC12" s="293"/>
+      <c r="BD12" s="293"/>
+      <c r="BE12" s="293"/>
+      <c r="BF12" s="293"/>
+      <c r="BG12" s="293"/>
+      <c r="BH12" s="293"/>
+      <c r="BI12" s="293"/>
+      <c r="BJ12" s="293"/>
+      <c r="BK12" s="293"/>
+      <c r="BL12" s="293"/>
+      <c r="BM12" s="293"/>
+      <c r="BN12" s="293"/>
+      <c r="BO12" s="293"/>
+      <c r="BP12" s="293"/>
+      <c r="BQ12" s="293"/>
+      <c r="BR12" s="293"/>
+      <c r="BS12" s="293"/>
+      <c r="BT12" s="293"/>
+      <c r="BU12" s="293"/>
+      <c r="BV12" s="293"/>
+      <c r="BW12" s="293"/>
+      <c r="BX12" s="293"/>
+      <c r="BY12" s="293"/>
+      <c r="BZ12" s="293"/>
+      <c r="CA12" s="293"/>
+      <c r="CB12" s="293"/>
+      <c r="CC12" s="293"/>
+      <c r="CD12" s="294"/>
     </row>
     <row r="13" spans="3:82" ht="15.75" customHeight="1">
       <c r="C13" s="122"/>
@@ -9918,12 +9916,12 @@
       <c r="G13" s="198"/>
       <c r="H13" s="199"/>
       <c r="I13" s="200"/>
-      <c r="J13" s="290"/>
-      <c r="K13" s="291"/>
-      <c r="L13" s="291"/>
-      <c r="M13" s="291"/>
-      <c r="N13" s="291"/>
-      <c r="O13" s="292"/>
+      <c r="J13" s="289"/>
+      <c r="K13" s="290"/>
+      <c r="L13" s="290"/>
+      <c r="M13" s="290"/>
+      <c r="N13" s="290"/>
+      <c r="O13" s="291"/>
       <c r="P13" s="46"/>
       <c r="Q13" s="47"/>
       <c r="R13" s="47"/>
@@ -9997,14 +9995,14 @@
       <c r="D14" s="122"/>
       <c r="E14" s="80"/>
       <c r="F14" s="81"/>
-      <c r="G14" s="267" t="s">
+      <c r="G14" s="266" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="268"/>
-      <c r="I14" s="268"/>
-      <c r="J14" s="268"/>
-      <c r="K14" s="268"/>
-      <c r="L14" s="269"/>
+      <c r="H14" s="267"/>
+      <c r="I14" s="267"/>
+      <c r="J14" s="267"/>
+      <c r="K14" s="267"/>
+      <c r="L14" s="268"/>
       <c r="M14" s="188" t="s">
         <v>35</v>
       </c>
@@ -10072,12 +10070,12 @@
       <c r="D15" s="122"/>
       <c r="E15" s="82"/>
       <c r="F15" s="83"/>
-      <c r="G15" s="270"/>
-      <c r="H15" s="271"/>
-      <c r="I15" s="271"/>
-      <c r="J15" s="271"/>
-      <c r="K15" s="271"/>
-      <c r="L15" s="272"/>
+      <c r="G15" s="269"/>
+      <c r="H15" s="270"/>
+      <c r="I15" s="270"/>
+      <c r="J15" s="270"/>
+      <c r="K15" s="270"/>
+      <c r="L15" s="271"/>
       <c r="M15" s="190"/>
       <c r="N15" s="35"/>
       <c r="O15" s="35"/>
@@ -10357,15 +10355,15 @@
       <c r="BF20" s="66"/>
       <c r="BG20" s="66"/>
       <c r="BH20" s="66"/>
-      <c r="BI20" s="264"/>
-      <c r="BJ20" s="265"/>
-      <c r="BK20" s="265"/>
-      <c r="BL20" s="265"/>
-      <c r="BM20" s="265"/>
-      <c r="BN20" s="265"/>
-      <c r="BO20" s="265"/>
-      <c r="BP20" s="265"/>
-      <c r="BQ20" s="266"/>
+      <c r="BI20" s="263"/>
+      <c r="BJ20" s="264"/>
+      <c r="BK20" s="264"/>
+      <c r="BL20" s="264"/>
+      <c r="BM20" s="264"/>
+      <c r="BN20" s="264"/>
+      <c r="BO20" s="264"/>
+      <c r="BP20" s="264"/>
+      <c r="BQ20" s="265"/>
       <c r="BS20" s="71"/>
       <c r="BT20" s="72"/>
       <c r="BU20" s="72"/>
@@ -10384,7 +10382,7 @@
       <c r="D21" s="122"/>
       <c r="E21" s="137"/>
       <c r="F21" s="138"/>
-      <c r="G21" s="273"/>
+      <c r="G21" s="272"/>
       <c r="H21" s="85"/>
       <c r="I21" s="172"/>
       <c r="J21" s="85"/>
@@ -10392,7 +10390,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="84"/>
       <c r="N21" s="85"/>
-      <c r="O21" s="273"/>
+      <c r="O21" s="272"/>
       <c r="P21" s="85"/>
       <c r="Q21" s="172"/>
       <c r="R21" s="85"/>
@@ -10400,7 +10398,7 @@
       <c r="T21" s="85"/>
       <c r="U21" s="84"/>
       <c r="V21" s="85"/>
-      <c r="W21" s="273"/>
+      <c r="W21" s="272"/>
       <c r="X21" s="85"/>
       <c r="Y21" s="172"/>
       <c r="Z21" s="85"/>
@@ -10476,7 +10474,7 @@
       <c r="D22" s="122"/>
       <c r="E22" s="137"/>
       <c r="F22" s="138"/>
-      <c r="G22" s="274"/>
+      <c r="G22" s="273"/>
       <c r="H22" s="85"/>
       <c r="I22" s="85"/>
       <c r="J22" s="85"/>
@@ -10484,7 +10482,7 @@
       <c r="L22" s="85"/>
       <c r="M22" s="86"/>
       <c r="N22" s="85"/>
-      <c r="O22" s="274"/>
+      <c r="O22" s="273"/>
       <c r="P22" s="85"/>
       <c r="Q22" s="85"/>
       <c r="R22" s="85"/>
@@ -10492,7 +10490,7 @@
       <c r="T22" s="85"/>
       <c r="U22" s="86"/>
       <c r="V22" s="85"/>
-      <c r="W22" s="274"/>
+      <c r="W22" s="273"/>
       <c r="X22" s="85"/>
       <c r="Y22" s="85"/>
       <c r="Z22" s="85"/>
@@ -11181,25 +11179,25 @@
     <row r="32" spans="3:102" ht="15.75" customHeight="1">
       <c r="C32" s="22"/>
       <c r="D32" s="12"/>
-      <c r="L32" s="262" t="s">
+      <c r="L32" s="261" t="s">
         <v>54</v>
       </c>
-      <c r="M32" s="262"/>
-      <c r="N32" s="262"/>
-      <c r="O32" s="262"/>
-      <c r="P32" s="262"/>
-      <c r="Q32" s="262"/>
-      <c r="R32" s="262"/>
-      <c r="S32" s="262"/>
-      <c r="T32" s="262"/>
-      <c r="U32" s="262"/>
-      <c r="V32" s="262"/>
-      <c r="W32" s="262"/>
-      <c r="X32" s="262"/>
-      <c r="Y32" s="262"/>
-      <c r="Z32" s="262"/>
-      <c r="AA32" s="262"/>
-      <c r="AB32" s="263"/>
+      <c r="M32" s="261"/>
+      <c r="N32" s="261"/>
+      <c r="O32" s="261"/>
+      <c r="P32" s="261"/>
+      <c r="Q32" s="261"/>
+      <c r="R32" s="261"/>
+      <c r="S32" s="261"/>
+      <c r="T32" s="261"/>
+      <c r="U32" s="261"/>
+      <c r="V32" s="261"/>
+      <c r="W32" s="261"/>
+      <c r="X32" s="261"/>
+      <c r="Y32" s="261"/>
+      <c r="Z32" s="261"/>
+      <c r="AA32" s="261"/>
+      <c r="AB32" s="262"/>
       <c r="AD32" s="4"/>
       <c r="AR32" s="245" t="s">
         <v>9</v>
@@ -11334,23 +11332,23 @@
       <c r="E34" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="296"/>
-      <c r="M34" s="296"/>
-      <c r="N34" s="296"/>
-      <c r="O34" s="296"/>
-      <c r="P34" s="296"/>
-      <c r="Q34" s="296"/>
-      <c r="R34" s="296"/>
-      <c r="S34" s="296"/>
-      <c r="T34" s="296"/>
-      <c r="U34" s="296"/>
-      <c r="V34" s="296"/>
-      <c r="W34" s="296"/>
-      <c r="X34" s="296"/>
-      <c r="Y34" s="296"/>
-      <c r="Z34" s="296"/>
-      <c r="AA34" s="296"/>
-      <c r="AB34" s="297"/>
+      <c r="L34" s="295"/>
+      <c r="M34" s="295"/>
+      <c r="N34" s="295"/>
+      <c r="O34" s="295"/>
+      <c r="P34" s="295"/>
+      <c r="Q34" s="295"/>
+      <c r="R34" s="295"/>
+      <c r="S34" s="295"/>
+      <c r="T34" s="295"/>
+      <c r="U34" s="295"/>
+      <c r="V34" s="295"/>
+      <c r="W34" s="295"/>
+      <c r="X34" s="295"/>
+      <c r="Y34" s="295"/>
+      <c r="Z34" s="295"/>
+      <c r="AA34" s="295"/>
+      <c r="AB34" s="296"/>
       <c r="AD34" s="137"/>
       <c r="AE34" s="249"/>
       <c r="AF34" s="23" t="s">
@@ -11408,21 +11406,21 @@
       <c r="E35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="261"/>
-      <c r="M35" s="261"/>
-      <c r="N35" s="261"/>
-      <c r="O35" s="261"/>
-      <c r="P35" s="261"/>
-      <c r="Q35" s="261"/>
-      <c r="R35" s="261"/>
-      <c r="S35" s="261"/>
-      <c r="T35" s="261"/>
-      <c r="U35" s="261"/>
-      <c r="V35" s="261"/>
-      <c r="W35" s="261"/>
-      <c r="X35" s="261"/>
-      <c r="Y35" s="261"/>
-      <c r="Z35" s="261"/>
+      <c r="L35" s="297"/>
+      <c r="M35" s="297"/>
+      <c r="N35" s="297"/>
+      <c r="O35" s="297"/>
+      <c r="P35" s="297"/>
+      <c r="Q35" s="297"/>
+      <c r="R35" s="297"/>
+      <c r="S35" s="297"/>
+      <c r="T35" s="297"/>
+      <c r="U35" s="297"/>
+      <c r="V35" s="297"/>
+      <c r="W35" s="297"/>
+      <c r="X35" s="297"/>
+      <c r="Y35" s="297"/>
+      <c r="Z35" s="297"/>
       <c r="AA35" s="24" t="s">
         <v>2</v>
       </c>
@@ -11872,7 +11870,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.39370078740157483" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>